<commit_message>
Updates to client documents from meeting; added new business dashboard design document
</commit_message>
<xml_diff>
--- a/docs/18 Reports from Data Base 6-5-2020 GRL.xlsx
+++ b/docs/18 Reports from Data Base 6-5-2020 GRL.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobgruhler\Documents\.1 Current Wild Cat Seed Fund\Data Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparlight\source\repos\Wildcatmicrofund\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AED909-4F29-4FA3-BF66-6DA8C890FC2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250"/>
+    <workbookView xWindow="27645" yWindow="360" windowWidth="10620" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>Wildcat Micro Fund</t>
   </si>
@@ -210,14 +213,28 @@
   </si>
   <si>
     <t>By Applicant - where in the process map are they?</t>
+  </si>
+  <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Will be a date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -245,8 +262,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,403 +544,419 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.36328125" customWidth="1"/>
-    <col min="3" max="3" width="3.6328125" customWidth="1"/>
-    <col min="4" max="4" width="3.453125" customWidth="1"/>
-    <col min="5" max="5" width="3.6328125" customWidth="1"/>
-    <col min="6" max="6" width="4.36328125" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="B48" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="B53" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="H57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="B60" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding client document modifications from meetings
</commit_message>
<xml_diff>
--- a/docs/18 Reports from Data Base 6-5-2020 GRL.xlsx
+++ b/docs/18 Reports from Data Base 6-5-2020 GRL.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobgruhler\Documents\.1 Current Wild Cat Seed Fund\Data Base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sparlight\source\repos\Wildcatmicrofund\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AED909-4F29-4FA3-BF66-6DA8C890FC2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250"/>
+    <workbookView xWindow="27645" yWindow="360" windowWidth="10620" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>Wildcat Micro Fund</t>
   </si>
@@ -210,14 +213,28 @@
   </si>
   <si>
     <t>By Applicant - where in the process map are they?</t>
+  </si>
+  <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Will be a date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -245,8 +262,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,403 +544,419 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.36328125" customWidth="1"/>
-    <col min="3" max="3" width="3.6328125" customWidth="1"/>
-    <col min="4" max="4" width="3.453125" customWidth="1"/>
-    <col min="5" max="5" width="3.6328125" customWidth="1"/>
-    <col min="6" max="6" width="4.36328125" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="B48" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="B53" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="H57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="B60" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>